<commit_message>
Alterações e ajustes nos documentos
</commit_message>
<xml_diff>
--- a/[Documentos]/Primeira Entrega/Mapa de Gantt.xlsx
+++ b/[Documentos]/Primeira Entrega/Mapa de Gantt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruajo\Documents\Aqua-Finder\[Documentos]\Primeira Entrega\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90925771-B630-4BB6-A76F-9A82D57A6CF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E1AFDD3-2523-4910-A56F-C438B79AFB0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>inicio</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t>Testes Finais</t>
+  </si>
+  <si>
+    <t>Encontrar bebedouros perto de Moscavide</t>
   </si>
 </sst>
 </file>
@@ -353,9 +356,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Folha1!$B$3:$B$19</c:f>
+              <c:f>Folha1!$B$3:$B$20</c:f>
               <c:strCache>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>Escolher o tema e nome</c:v>
                 </c:pt>
@@ -381,30 +384,33 @@
                   <c:v>PRIMEIRA ENTREGA</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>Encontrar bebedouros perto de Moscavide</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>Desenvolvimento do back-end</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>Desenvolvimento do front-end</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>SEGUNDA ENTREGA</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>Desenvolvimento do back-end</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>Desenvolvimento do front-end</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>Fase de testes</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>Ajustes Finais</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>Testes Finais</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>TERCEIRA ENTREGA</c:v>
                 </c:pt>
               </c:strCache>
@@ -412,10 +418,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Folha1!$C$3:$C$19</c:f>
+              <c:f>Folha1!$C$3:$C$20</c:f>
               <c:numCache>
                 <c:formatCode>[$-816]d/mmm;@</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>45916</c:v>
                 </c:pt>
@@ -447,24 +453,27 @@
                   <c:v>45928</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>45928</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>45970</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>45993</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>46003</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>45928</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>45928</c:v>
                 </c:pt>
                 <c:pt idx="15">
+                  <c:v>45928</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>45993</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>46005</c:v>
                 </c:pt>
               </c:numCache>
@@ -564,9 +573,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Folha1!$B$3:$B$19</c:f>
+              <c:f>Folha1!$B$3:$B$20</c:f>
               <c:strCache>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>Escolher o tema e nome</c:v>
                 </c:pt>
@@ -592,30 +601,33 @@
                   <c:v>PRIMEIRA ENTREGA</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>Encontrar bebedouros perto de Moscavide</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>Desenvolvimento do back-end</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>Desenvolvimento do front-end</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>SEGUNDA ENTREGA</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>Desenvolvimento do back-end</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>Desenvolvimento do front-end</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>Fase de testes</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>Ajustes Finais</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>Testes Finais</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>TERCEIRA ENTREGA</c:v>
                 </c:pt>
               </c:strCache>
@@ -623,10 +635,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Folha1!$D$3:$D$19</c:f>
+              <c:f>Folha1!$D$3:$D$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -652,30 +664,33 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>50</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>65</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>50</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>65</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -711,9 +726,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Folha1!$B$3:$B$19</c:f>
+              <c:f>Folha1!$B$3:$B$20</c:f>
               <c:strCache>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>Escolher o tema e nome</c:v>
                 </c:pt>
@@ -739,30 +754,33 @@
                   <c:v>PRIMEIRA ENTREGA</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>Encontrar bebedouros perto de Moscavide</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>Desenvolvimento do back-end</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>Desenvolvimento do front-end</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>SEGUNDA ENTREGA</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>Desenvolvimento do back-end</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>Desenvolvimento do front-end</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>Fase de testes</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>Ajustes Finais</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>Testes Finais</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>TERCEIRA ENTREGA</c:v>
                 </c:pt>
               </c:strCache>
@@ -770,10 +788,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Folha1!$D$3:$D$19</c:f>
+              <c:f>Folha1!$D$3:$D$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -799,30 +817,33 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>50</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>65</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>50</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>65</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -1922,8 +1943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="76" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="Q59" sqref="Q59"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="77" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2024,7 +2045,7 @@
         <v>85</v>
       </c>
       <c r="E7" s="4">
-        <f t="shared" ref="E7:E20" si="1">C7+D7</f>
+        <f t="shared" ref="E7:E10" si="1">C7+D7</f>
         <v>46005</v>
       </c>
     </row>
@@ -2075,151 +2096,166 @@
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C11" s="7">
         <v>45928</v>
       </c>
       <c r="D11" s="1">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="E11" s="4">
-        <f t="shared" si="1"/>
-        <v>45978</v>
+        <f>C11+D11</f>
+        <v>45933</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C12" s="7">
         <v>45928</v>
       </c>
       <c r="D12" s="1">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="E12" s="4">
-        <f t="shared" si="1"/>
-        <v>45993</v>
+        <f>C12+D12</f>
+        <v>45978</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B13" s="12" t="s">
-        <v>18</v>
+      <c r="B13" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="C13" s="7">
-        <v>45970</v>
+        <v>45928</v>
       </c>
       <c r="D13" s="1">
-        <v>1</v>
+        <v>65</v>
       </c>
       <c r="E13" s="4">
-        <f t="shared" si="1"/>
-        <v>45971</v>
+        <f>C13+D13</f>
+        <v>45993</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="8">
-        <v>45993</v>
+      <c r="B14" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="7">
+        <v>45970</v>
       </c>
       <c r="D14" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E14" s="4">
-        <f t="shared" si="1"/>
-        <v>46003</v>
+        <f>C14+D14</f>
+        <v>45971</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C15" s="8">
+        <v>45993</v>
+      </c>
+      <c r="D15" s="1">
+        <v>10</v>
+      </c>
+      <c r="E15" s="4">
+        <f>C15+D15</f>
         <v>46003</v>
-      </c>
-      <c r="D15" s="1">
-        <v>4</v>
-      </c>
-      <c r="E15" s="4">
-        <f t="shared" si="1"/>
-        <v>46007</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="7">
-        <v>45928</v>
+        <v>12</v>
+      </c>
+      <c r="C16" s="8">
+        <v>46003</v>
       </c>
       <c r="D16" s="1">
-        <v>50</v>
+        <v>4</v>
       </c>
       <c r="E16" s="4">
-        <f t="shared" si="1"/>
-        <v>45978</v>
+        <f>C16+D16</f>
+        <v>46007</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C17" s="7">
         <v>45928</v>
       </c>
       <c r="D17" s="1">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="E17" s="4">
-        <f t="shared" si="1"/>
-        <v>45993</v>
+        <f>C17+D17</f>
+        <v>45978</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="8">
+        <v>21</v>
+      </c>
+      <c r="C18" s="7">
+        <v>45928</v>
+      </c>
+      <c r="D18" s="1">
+        <v>65</v>
+      </c>
+      <c r="E18" s="4">
+        <f>C18+D18</f>
         <v>45993</v>
-      </c>
-      <c r="D18" s="1">
-        <v>10</v>
-      </c>
-      <c r="E18" s="4">
-        <f t="shared" si="1"/>
-        <v>46003</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B19" s="12" t="s">
-        <v>19</v>
+      <c r="B19" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="C19" s="8">
-        <v>46005</v>
+        <v>45993</v>
       </c>
       <c r="D19" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E19" s="4">
-        <f t="shared" si="1"/>
-        <v>46006</v>
+        <f>C19+D19</f>
+        <v>46003</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="8">
+        <v>46005</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1</v>
+      </c>
+      <c r="E20" s="4">
+        <f>C20+D20</f>
+        <v>46006</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B21" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="8">
+      <c r="C21" s="8">
         <v>46003</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D21" s="1">
         <v>4</v>
       </c>
-      <c r="E20" s="4">
-        <f t="shared" si="1"/>
+      <c r="E21" s="4">
+        <f>C21+D21</f>
         <v>46007</v>
       </c>
     </row>
@@ -2237,7 +2273,7 @@
         <v>4</v>
       </c>
       <c r="C27" s="5">
-        <f>E19</f>
+        <f>E20</f>
         <v>46006</v>
       </c>
     </row>
@@ -2284,15 +2320,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101002E0C5F17F802A944A64A28E7E34948C2" ma:contentTypeVersion="14" ma:contentTypeDescription="Criar um novo documento." ma:contentTypeScope="" ma:versionID="b3b31ff88e898c792e30bcd40b7d5c56">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="db72107c-c97d-424d-9d7a-20ff74df8ad9" xmlns:ns3="cbc7956b-1ba7-4aac-a59d-60d58a1d6fec" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dc794439361061b5e64cfae82a24d306" ns2:_="" ns3:_="">
     <xsd:import namespace="db72107c-c97d-424d-9d7a-20ff74df8ad9"/>
@@ -2521,6 +2548,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5EBBA12-ED3E-4F5E-9D94-22616A017D82}">
   <ds:schemaRefs>
@@ -2533,14 +2569,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E735A985-0F61-4E63-9E63-0641CB4FC096}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4D9D28A-8FDC-4B09-ACB5-C096BC2F9E9A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2557,4 +2585,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E735A985-0F61-4E63-9E63-0641CB4FC096}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Ajustes no mapa de gantt, relatorio, criação da apresentação e readme
</commit_message>
<xml_diff>
--- a/[Documentos]/Primeira Entrega/Mapa de Gantt.xlsx
+++ b/[Documentos]/Primeira Entrega/Mapa de Gantt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruajo\Documents\Aqua-Finder\[Documentos]\Primeira Entrega\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E1AFDD3-2523-4910-A56F-C438B79AFB0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED0238D2-090E-4968-A58B-785597FF85B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -444,34 +444,34 @@
                   <c:v>45920</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>45928</c:v>
+                  <c:v>45935</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>45928</c:v>
+                  <c:v>45936</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>45928</c:v>
+                  <c:v>45938</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>45928</c:v>
+                  <c:v>45938</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>45970</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>45993</c:v>
+                  <c:v>45970</c:v>
                 </c:pt>
                 <c:pt idx="13">
+                  <c:v>45970</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>46000</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>46003</c:v>
                 </c:pt>
-                <c:pt idx="14">
-                  <c:v>45928</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>45928</c:v>
-                </c:pt>
                 <c:pt idx="16">
-                  <c:v>45993</c:v>
+                  <c:v>46004</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>46005</c:v>
@@ -667,28 +667,28 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>50</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>65</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>10</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>50</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>65</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>10</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>1</c:v>
@@ -820,28 +820,28 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>50</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>65</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>10</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>50</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>65</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>10</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>1</c:v>
@@ -1620,11 +1620,11 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>263523</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>52068</xdr:rowOff>
+      <xdr:rowOff>65690</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>296882</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>118242</xdr:colOff>
       <xdr:row>57</xdr:row>
       <xdr:rowOff>158337</xdr:rowOff>
     </xdr:to>
@@ -1943,24 +1943,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="77" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" customWidth="1"/>
-    <col min="2" max="2" width="49.5546875" customWidth="1"/>
-    <col min="3" max="3" width="24.44140625" customWidth="1"/>
-    <col min="5" max="5" width="24.6640625" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" customWidth="1"/>
+    <col min="2" max="2" width="49.5703125" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1974,7 +1974,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
@@ -1989,7 +1989,7 @@
         <v>45918</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
@@ -2004,7 +2004,7 @@
         <v>45926</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
@@ -2019,7 +2019,7 @@
         <v>45926</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
@@ -2034,7 +2034,7 @@
         <v>45925</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
@@ -2049,7 +2049,7 @@
         <v>46005</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
@@ -2064,7 +2064,7 @@
         <v>45927</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
@@ -2079,67 +2079,67 @@
         <v>45927</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="12" t="s">
         <v>17</v>
       </c>
       <c r="C10" s="7">
-        <v>45928</v>
+        <v>45935</v>
       </c>
       <c r="D10" s="1">
         <v>1</v>
       </c>
       <c r="E10" s="4">
         <f t="shared" si="1"/>
-        <v>45929</v>
+        <v>45936</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C11" s="7">
-        <v>45928</v>
+        <v>45936</v>
       </c>
       <c r="D11" s="1">
         <v>5</v>
       </c>
       <c r="E11" s="4">
-        <f>C11+D11</f>
-        <v>45933</v>
+        <f t="shared" ref="E11:E21" si="2">C11+D11</f>
+        <v>45941</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C12" s="7">
-        <v>45928</v>
+        <v>45938</v>
       </c>
       <c r="D12" s="1">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="E12" s="4">
-        <f>C12+D12</f>
-        <v>45978</v>
+        <f t="shared" si="2"/>
+        <v>45969</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="7">
-        <v>45928</v>
+        <v>45938</v>
       </c>
       <c r="D13" s="1">
-        <v>65</v>
+        <v>31</v>
       </c>
       <c r="E13" s="4">
-        <f>C13+D13</f>
-        <v>45993</v>
+        <f t="shared" si="2"/>
+        <v>45969</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="12" t="s">
         <v>18</v>
       </c>
@@ -2150,86 +2150,86 @@
         <v>1</v>
       </c>
       <c r="E14" s="4">
-        <f>C14+D14</f>
+        <f t="shared" si="2"/>
         <v>45971</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="8">
-        <v>45993</v>
+        <v>45970</v>
       </c>
       <c r="D15" s="1">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="E15" s="4">
-        <f>C15+D15</f>
-        <v>46003</v>
+        <f t="shared" si="2"/>
+        <v>46000</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C16" s="8">
-        <v>46003</v>
+        <v>45970</v>
       </c>
       <c r="D16" s="1">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="E16" s="4">
-        <f>C16+D16</f>
-        <v>46007</v>
+        <f t="shared" si="2"/>
+        <v>46000</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C17" s="7">
-        <v>45928</v>
+        <v>46000</v>
       </c>
       <c r="D17" s="1">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="E17" s="4">
-        <f>C17+D17</f>
-        <v>45978</v>
+        <f t="shared" si="2"/>
+        <v>46003</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C18" s="7">
-        <v>45928</v>
+        <v>46003</v>
       </c>
       <c r="D18" s="1">
-        <v>65</v>
+        <v>1</v>
       </c>
       <c r="E18" s="4">
-        <f>C18+D18</f>
-        <v>45993</v>
+        <f t="shared" si="2"/>
+        <v>46004</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C19" s="8">
-        <v>45993</v>
+        <v>46004</v>
       </c>
       <c r="D19" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E19" s="4">
-        <f>C19+D19</f>
-        <v>46003</v>
+        <f t="shared" si="2"/>
+        <v>46005</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="12" t="s">
         <v>19</v>
       </c>
@@ -2240,11 +2240,11 @@
         <v>1</v>
       </c>
       <c r="E20" s="4">
-        <f>C20+D20</f>
+        <f t="shared" si="2"/>
         <v>46006</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>3</v>
       </c>
@@ -2255,11 +2255,11 @@
         <v>4</v>
       </c>
       <c r="E21" s="4">
-        <f>C21+D21</f>
+        <f t="shared" si="2"/>
         <v>46007</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="6" t="s">
         <v>0</v>
       </c>
@@ -2268,7 +2268,7 @@
         <v>45918</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="6" t="s">
         <v>4</v>
       </c>
@@ -2290,7 +2290,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2302,7 +2302,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>